<commit_message>
SE-2339: Add uploading simple instruments example.
</commit_message>
<xml_diff>
--- a/examples/lusid/instruments/_data/instruments.xlsx
+++ b/examples/lusid/instruments/_data/instruments.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\gl\luminesce-examples\examples\lusid\instruments\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatthewFox\work\code\luminesce-examples\luminesce-examples\examples\lusid\instruments\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE567794-EDB7-4615-AF3B-8ACA7E4EBB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFEAC6F3-EC94-4FFD-92E5-96DC115C3021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2076" yWindow="1638" windowWidth="18660" windowHeight="10722" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equities" sheetId="1" r:id="rId1"/>
     <sheet name="term_deposits" sheetId="2" r:id="rId2"/>
+    <sheet name="simple_instruments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="544">
   <si>
     <t>Ticker</t>
   </si>
@@ -1631,6 +1632,33 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Equities</t>
+  </si>
+  <si>
+    <t>Equity</t>
+  </si>
+  <si>
+    <t>GBP Cash</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Cash</t>
+  </si>
+  <si>
+    <t>CCYGBP</t>
   </si>
 </sst>
 </file>
@@ -1952,7 +1980,7 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3994,7 +4022,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D55F91E-4EE6-4093-B9EA-FF8B098131BE}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4192,4 +4220,230 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6321120-EF00-40A5-ABF3-4EE7933E7603}">
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="15.83984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7890625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" t="s">
+        <v>512</v>
+      </c>
+      <c r="D2" t="s">
+        <v>538</v>
+      </c>
+      <c r="E2" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D3" t="s">
+        <v>538</v>
+      </c>
+      <c r="E3" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D4" t="s">
+        <v>538</v>
+      </c>
+      <c r="E4" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" t="s">
+        <v>512</v>
+      </c>
+      <c r="D5" t="s">
+        <v>538</v>
+      </c>
+      <c r="E5" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>213</v>
+      </c>
+      <c r="B6" t="s">
+        <v>215</v>
+      </c>
+      <c r="C6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D6" t="s">
+        <v>538</v>
+      </c>
+      <c r="E6" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C7" t="s">
+        <v>512</v>
+      </c>
+      <c r="D7" t="s">
+        <v>538</v>
+      </c>
+      <c r="E7" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" t="s">
+        <v>478</v>
+      </c>
+      <c r="B8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C8" t="s">
+        <v>512</v>
+      </c>
+      <c r="D8" t="s">
+        <v>538</v>
+      </c>
+      <c r="E8" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" t="s">
+        <v>376</v>
+      </c>
+      <c r="B9" t="s">
+        <v>379</v>
+      </c>
+      <c r="C9" t="s">
+        <v>512</v>
+      </c>
+      <c r="D9" t="s">
+        <v>538</v>
+      </c>
+      <c r="E9" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" t="s">
+        <v>493</v>
+      </c>
+      <c r="B10" t="s">
+        <v>497</v>
+      </c>
+      <c r="C10" t="s">
+        <v>512</v>
+      </c>
+      <c r="D10" t="s">
+        <v>538</v>
+      </c>
+      <c r="E10" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>512</v>
+      </c>
+      <c r="D11" t="s">
+        <v>538</v>
+      </c>
+      <c r="E11" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" t="s">
+        <v>540</v>
+      </c>
+      <c r="B12" t="s">
+        <v>543</v>
+      </c>
+      <c r="C12" t="s">
+        <v>512</v>
+      </c>
+      <c r="D12" t="s">
+        <v>541</v>
+      </c>
+      <c r="E12" t="s">
+        <v>542</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
SE-2339: Add simple instrument data.
</commit_message>
<xml_diff>
--- a/examples/lusid/instruments/_data/instruments.xlsx
+++ b/examples/lusid/instruments/_data/instruments.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\gl\luminesce-examples\examples\lusid\instruments\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatthewFox\work\code\luminesce-examples\luminesce-examples\examples\lusid\instruments\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE567794-EDB7-4615-AF3B-8ACA7E4EBB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9FF0549-55EA-4DC3-A2E3-74BD192DD659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2076" yWindow="2196" windowWidth="18660" windowHeight="10722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equities" sheetId="1" r:id="rId1"/>
     <sheet name="term_deposits" sheetId="2" r:id="rId2"/>
+    <sheet name="simple_instruments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="550">
   <si>
     <t>Ticker</t>
   </si>
@@ -1631,6 +1632,51 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>LondonShoppingCentre</t>
+  </si>
+  <si>
+    <t>BirminghamShoppingCentre</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>ShoppingCentres</t>
+  </si>
+  <si>
+    <t>SHOPCENCI1</t>
+  </si>
+  <si>
+    <t>SHOPCENCI2</t>
+  </si>
+  <si>
+    <t>SHOPCENCI3</t>
+  </si>
+  <si>
+    <t>SHOPCENCI4</t>
+  </si>
+  <si>
+    <t>SHOPCENCI5</t>
+  </si>
+  <si>
+    <t>OxfordShoppingCentre</t>
+  </si>
+  <si>
+    <t>BathShoppingCentre</t>
+  </si>
+  <si>
+    <t>WarwickShoppingCentre</t>
   </si>
 </sst>
 </file>
@@ -1951,16 +1997,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.41796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.68359375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3994,7 +4040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D55F91E-4EE6-4093-B9EA-FF8B098131BE}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4003,13 +4049,13 @@
     <col min="1" max="1" width="11.26171875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.41796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.9453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.68359375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.41796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.68359375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4192,4 +4238,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6321120-EF00-40A5-ABF3-4EE7933E7603}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="26.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C2" t="s">
+        <v>512</v>
+      </c>
+      <c r="D2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D3" t="s">
+        <v>540</v>
+      </c>
+      <c r="E3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>547</v>
+      </c>
+      <c r="B4" t="s">
+        <v>544</v>
+      </c>
+      <c r="C4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D4" t="s">
+        <v>540</v>
+      </c>
+      <c r="E4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B5" t="s">
+        <v>545</v>
+      </c>
+      <c r="C5" t="s">
+        <v>512</v>
+      </c>
+      <c r="D5" t="s">
+        <v>540</v>
+      </c>
+      <c r="E5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D6" t="s">
+        <v>540</v>
+      </c>
+      <c r="E6" t="s">
+        <v>541</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Feature/se 2339.simple instrument luminesce example (#36)
* SE-2339: Add simple instrument data.

* SE-2339: Add upload and get instrument examples.

* SE-2342: Reformat to match other examples.

Co-authored-by: Matthew Fox <matthew.fox@finbourne.com>
</commit_message>
<xml_diff>
--- a/examples/lusid/instruments/_data/instruments.xlsx
+++ b/examples/lusid/instruments/_data/instruments.xlsx
@@ -5,16 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\code\gl\luminesce-examples\examples\lusid\instruments\_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MatthewFox\work\code\luminesce-examples\luminesce-examples\examples\lusid\instruments\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE567794-EDB7-4615-AF3B-8ACA7E4EBB78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9FF0549-55EA-4DC3-A2E3-74BD192DD659}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2076" yWindow="2196" windowWidth="18660" windowHeight="10722" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equities" sheetId="1" r:id="rId1"/>
     <sheet name="term_deposits" sheetId="2" r:id="rId2"/>
+    <sheet name="simple_instruments" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="535">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="550">
   <si>
     <t>Ticker</t>
   </si>
@@ -1631,6 +1632,51 @@
   </si>
   <si>
     <t>currency</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>LondonShoppingCentre</t>
+  </si>
+  <si>
+    <t>BirminghamShoppingCentre</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>ShoppingCentres</t>
+  </si>
+  <si>
+    <t>SHOPCENCI1</t>
+  </si>
+  <si>
+    <t>SHOPCENCI2</t>
+  </si>
+  <si>
+    <t>SHOPCENCI3</t>
+  </si>
+  <si>
+    <t>SHOPCENCI4</t>
+  </si>
+  <si>
+    <t>SHOPCENCI5</t>
+  </si>
+  <si>
+    <t>OxfordShoppingCentre</t>
+  </si>
+  <si>
+    <t>BathShoppingCentre</t>
+  </si>
+  <si>
+    <t>WarwickShoppingCentre</t>
   </si>
 </sst>
 </file>
@@ -1951,16 +1997,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="8.1015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.15625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.3125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.47265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.41796875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="16.68359375" bestFit="1" customWidth="1"/>
   </cols>
@@ -3994,7 +4040,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D55F91E-4EE6-4093-B9EA-FF8B098131BE}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -4003,13 +4049,13 @@
     <col min="1" max="1" width="11.26171875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.41796875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.26171875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.9453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="30.578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="25.68359375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="28.41796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.68359375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -4192,4 +4238,128 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6321120-EF00-40A5-ABF3-4EE7933E7603}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I6" sqref="I6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="26.578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.68359375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.41796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.26171875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>535</v>
+      </c>
+      <c r="D1" t="s">
+        <v>536</v>
+      </c>
+      <c r="E1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" t="s">
+        <v>538</v>
+      </c>
+      <c r="B2" t="s">
+        <v>542</v>
+      </c>
+      <c r="C2" t="s">
+        <v>512</v>
+      </c>
+      <c r="D2" t="s">
+        <v>540</v>
+      </c>
+      <c r="E2" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" t="s">
+        <v>539</v>
+      </c>
+      <c r="B3" t="s">
+        <v>543</v>
+      </c>
+      <c r="C3" t="s">
+        <v>512</v>
+      </c>
+      <c r="D3" t="s">
+        <v>540</v>
+      </c>
+      <c r="E3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>547</v>
+      </c>
+      <c r="B4" t="s">
+        <v>544</v>
+      </c>
+      <c r="C4" t="s">
+        <v>512</v>
+      </c>
+      <c r="D4" t="s">
+        <v>540</v>
+      </c>
+      <c r="E4" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" t="s">
+        <v>548</v>
+      </c>
+      <c r="B5" t="s">
+        <v>545</v>
+      </c>
+      <c r="C5" t="s">
+        <v>512</v>
+      </c>
+      <c r="D5" t="s">
+        <v>540</v>
+      </c>
+      <c r="E5" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" t="s">
+        <v>549</v>
+      </c>
+      <c r="B6" t="s">
+        <v>546</v>
+      </c>
+      <c r="C6" t="s">
+        <v>512</v>
+      </c>
+      <c r="D6" t="s">
+        <v>540</v>
+      </c>
+      <c r="E6" t="s">
+        <v>541</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>